<commit_message>
Use logging to replace all prints.
</commit_message>
<xml_diff>
--- a/experiment_comparison/df_DAL_UE_avg_major_100.xlsx
+++ b/experiment_comparison/df_DAL_UE_avg_major_100.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>AL_SQP</t>
+          <t>AL-SQP</t>
         </is>
       </c>
     </row>
@@ -465,19 +465,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>482.842457858034</v>
+        <v>493.2489079521391</v>
       </c>
       <c r="C2" t="n">
-        <v>428.2625729380858</v>
+        <v>398.0125759009749</v>
       </c>
       <c r="D2" t="n">
-        <v>482.8424578580339</v>
+        <v>489.6521082785899</v>
       </c>
       <c r="E2" t="n">
-        <v>426.3783440677448</v>
+        <v>411.9903044170762</v>
       </c>
       <c r="F2" t="n">
-        <v>491.1828446091903</v>
+        <v>498.5425510850154</v>
       </c>
     </row>
     <row r="3">
@@ -485,19 +485,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>478.4382157549788</v>
+        <v>490.92598839141</v>
       </c>
       <c r="C3" t="n">
-        <v>412.2882903185599</v>
+        <v>420.1427919264566</v>
       </c>
       <c r="D3" t="n">
-        <v>478.4382157549788</v>
+        <v>493.364789575227</v>
       </c>
       <c r="E3" t="n">
-        <v>405.3120544690073</v>
+        <v>403.6789918291935</v>
       </c>
       <c r="F3" t="n">
-        <v>483.7902505975075</v>
+        <v>499.5835623833169</v>
       </c>
     </row>
     <row r="4">
@@ -505,19 +505,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>495.946473746524</v>
+        <v>486.5966483399661</v>
       </c>
       <c r="C4" t="n">
-        <v>436.6766587283622</v>
+        <v>359.1921061179575</v>
       </c>
       <c r="D4" t="n">
-        <v>495.9464737465241</v>
+        <v>491.2368821989236</v>
       </c>
       <c r="E4" t="n">
-        <v>435.1522896946652</v>
+        <v>283.4839307807926</v>
       </c>
       <c r="F4" t="n">
-        <v>500.0417943235911</v>
+        <v>495.0859409474938</v>
       </c>
     </row>
     <row r="5">
@@ -525,19 +525,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>488.483731352553</v>
+        <v>466.6824725294445</v>
       </c>
       <c r="C5" t="n">
-        <v>420.3091330644776</v>
+        <v>398.9847710574171</v>
       </c>
       <c r="D5" t="n">
-        <v>488.483731352553</v>
+        <v>477.0345653802399</v>
       </c>
       <c r="E5" t="n">
-        <v>398.0974509897085</v>
+        <v>389.2410313257318</v>
       </c>
       <c r="F5" t="n">
-        <v>490.8972893050468</v>
+        <v>479.2495412993596</v>
       </c>
     </row>
     <row r="6">
@@ -545,19 +545,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>491.2488870854783</v>
+        <v>465.4623654255223</v>
       </c>
       <c r="C6" t="n">
-        <v>421.7378419241055</v>
+        <v>364.838061883233</v>
       </c>
       <c r="D6" t="n">
-        <v>491.2488870854783</v>
+        <v>480.2212943784397</v>
       </c>
       <c r="E6" t="n">
-        <v>389.9532717646877</v>
+        <v>334.1144620973773</v>
       </c>
       <c r="F6" t="n">
-        <v>494.0678201212837</v>
+        <v>483.4524913894659</v>
       </c>
     </row>
     <row r="7">
@@ -565,19 +565,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>489.4556658169478</v>
+        <v>452.6495762701873</v>
       </c>
       <c r="C7" t="n">
-        <v>418.9320342573774</v>
+        <v>364.8549915166554</v>
       </c>
       <c r="D7" t="n">
-        <v>489.4556658169478</v>
+        <v>471.4130381358773</v>
       </c>
       <c r="E7" t="n">
-        <v>402.7477970815908</v>
+        <v>391.4503704283915</v>
       </c>
       <c r="F7" t="n">
-        <v>493.468766691565</v>
+        <v>475.007333934248</v>
       </c>
     </row>
     <row r="8">
@@ -585,19 +585,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>487.244090940553</v>
+        <v>472.3969636003201</v>
       </c>
       <c r="C8" t="n">
-        <v>412.6346395729671</v>
+        <v>403.881023021193</v>
       </c>
       <c r="D8" t="n">
-        <v>487.2440909405529</v>
+        <v>494.9636192133948</v>
       </c>
       <c r="E8" t="n">
-        <v>397.0877201925517</v>
+        <v>390.1819007836912</v>
       </c>
       <c r="F8" t="n">
-        <v>490.1807417820231</v>
+        <v>497.9661947390633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>